<commit_message>
Part 5 Submission 2: Added Test Scenarios
</commit_message>
<xml_diff>
--- a/Technocrats University Requirement Tracability Matrix and Cases.xlsx
+++ b/Technocrats University Requirement Tracability Matrix and Cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="82">
   <si>
     <t>Business Requirement</t>
   </si>
@@ -160,9 +160,6 @@
     <t>Verify inputting ID leads to correct student being displayed</t>
   </si>
   <si>
-    <t>id=1</t>
-  </si>
-  <si>
     <t>Displayed student is correct</t>
   </si>
   <si>
@@ -263,6 +260,60 @@
   </si>
   <si>
     <t>Source: Adapted from Guru 99 templates for RTM</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Verify functionality of All Majors page</t>
+  </si>
+  <si>
+    <t>Make sure that page displays all available majors</t>
+  </si>
+  <si>
+    <t>5
+6</t>
+  </si>
+  <si>
+    <t>Verify functionality of All Students page</t>
+  </si>
+  <si>
+    <t>Make sure that page displays all students</t>
+  </si>
+  <si>
+    <t>1
+2</t>
+  </si>
+  <si>
+    <t>Verify functionality of Get Major By ID page</t>
+  </si>
+  <si>
+    <t>Make sure that page displays major when ID is submitted, that improper IDs do not crash the page, and that going directly to the view page will not crash</t>
+  </si>
+  <si>
+    <t>7
+8</t>
+  </si>
+  <si>
+    <t>Verify functionality of Get Student By ID page</t>
+  </si>
+  <si>
+    <t>Make sure that page displays student when ID is submitted, that improper IDs do not crash the page, and that going directly to the view page will not crash</t>
+  </si>
+  <si>
+    <t>3
+4</t>
+  </si>
+  <si>
+    <t>Test Scenario Number</t>
+  </si>
+  <si>
+    <t>id=1
+id=-1
+id='a'</t>
   </si>
 </sst>
 </file>
@@ -599,15 +650,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="141" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="76.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
@@ -785,313 +838,410 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="1" t="s">
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="E28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="1">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
         <v>5</v>
       </c>
-      <c r="B22" s="1" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="B39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
         <v>6</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="1">
+        <v>3</v>
+      </c>
+      <c r="D40" s="1">
         <v>7</v>
       </c>
-      <c r="B24" s="1" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="B41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="1">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1">
         <v>8</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>66</v>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>